<commit_message>
created RAW file. made removed some non-english articles from cleaned
</commit_message>
<xml_diff>
--- a/generated claim ver/russia_claims.xlsx
+++ b/generated claim ver/russia_claims.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,37 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>supporting</t>
+          <t>high_supporting</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>rejecting</t>
+          <t>high_rejecting</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>med_supporting</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>med_rejecting</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>supporting_count</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>neutral_count</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>rejecting_count</t>
         </is>
       </c>
     </row>
@@ -469,6 +494,25 @@
           <t>[]</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>['russia_19', 'russia_89', 'russia_189']</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" t="n">
+        <v>326</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -481,13 +525,32 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['russia_46', 'russia_92', 'russia_97', 'russia_209', 'russia_231', 'russia_335', 'russia_359', 'russia_407', 'russia_464']</t>
+          <t>['russia_46', 'russia_92', 'russia_97', 'russia_209', 'russia_231', 'russia_359']</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>['russia_38', 'russia_118', 'russia_297', 'russia_335', 'russia_350', 'russia_388', 'russia_407', 'russia_437', 'russia_440', 'russia_464']</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>16</v>
+      </c>
+      <c r="H3" t="n">
+        <v>330</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -501,13 +564,32 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['russia_19', 'russia_26', 'russia_28', 'russia_50', 'russia_66', 'russia_68', 'russia_97', 'russia_105', 'russia_118', 'russia_138', 'russia_214', 'russia_217', 'russia_233', 'russia_238', 'russia_281', 'russia_322', 'russia_330', 'russia_339', 'russia_342', 'russia_348', 'russia_351', 'russia_357', 'russia_409', 'russia_458', 'russia_475', 'russia_483']</t>
+          <t>['russia_19', 'russia_50', 'russia_66', 'russia_97', 'russia_118', 'russia_138', 'russia_238', 'russia_322', 'russia_342', 'russia_351', 'russia_357', 'russia_458', 'russia_483']</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['russia_8', 'russia_20', 'russia_23', 'russia_29', 'russia_35', 'russia_48', 'russia_51', 'russia_57', 'russia_61', 'russia_69', 'russia_74', 'russia_81', 'russia_108', 'russia_112', 'russia_114', 'russia_117', 'russia_132', 'russia_154', 'russia_156', 'russia_175', 'russia_176', 'russia_180', 'russia_181', 'russia_212', 'russia_213', 'russia_219', 'russia_220', 'russia_234', 'russia_240', 'russia_252', 'russia_266', 'russia_271', 'russia_273', 'russia_274', 'russia_279', 'russia_300', 'russia_305', 'russia_310', 'russia_315', 'russia_316', 'russia_321', 'russia_323', 'russia_344', 'russia_363', 'russia_364', 'russia_368', 'russia_369', 'russia_399', 'russia_401', 'russia_413', 'russia_415', 'russia_416', 'russia_433', 'russia_440', 'russia_497']</t>
-        </is>
+          <t>['russia_29', 'russia_35', 'russia_48', 'russia_57', 'russia_61', 'russia_69', 'russia_108', 'russia_112', 'russia_114', 'russia_117', 'russia_154', 'russia_176', 'russia_180', 'russia_181', 'russia_212', 'russia_219', 'russia_252', 'russia_300', 'russia_305', 'russia_321', 'russia_323', 'russia_363', 'russia_364', 'russia_368', 'russia_369', 'russia_416']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>['russia_13', 'russia_14', 'russia_26', 'russia_28', 'russia_40', 'russia_46', 'russia_68', 'russia_89', 'russia_105', 'russia_115', 'russia_119', 'russia_152', 'russia_187', 'russia_188', 'russia_192', 'russia_194', 'russia_198', 'russia_214', 'russia_217', 'russia_233', 'russia_235', 'russia_239', 'russia_242', 'russia_254', 'russia_277', 'russia_281', 'russia_298', 'russia_330', 'russia_339', 'russia_340', 'russia_341', 'russia_345', 'russia_347', 'russia_348', 'russia_349', 'russia_372', 'russia_377', 'russia_383', 'russia_384', 'russia_409', 'russia_437', 'russia_459', 'russia_475']</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>['russia_4', 'russia_8', 'russia_20', 'russia_23', 'russia_24', 'russia_25', 'russia_38', 'russia_43', 'russia_51', 'russia_62', 'russia_63', 'russia_70', 'russia_72', 'russia_74', 'russia_80', 'russia_81', 'russia_93', 'russia_94', 'russia_99', 'russia_132', 'russia_137', 'russia_141', 'russia_149', 'russia_156', 'russia_158', 'russia_175', 'russia_196', 'russia_210', 'russia_213', 'russia_220', 'russia_224', 'russia_231', 'russia_234', 'russia_240', 'russia_262', 'russia_266', 'russia_271', 'russia_273', 'russia_274', 'russia_279', 'russia_287', 'russia_293', 'russia_294', 'russia_296', 'russia_303', 'russia_306', 'russia_309', 'russia_310', 'russia_313', 'russia_315', 'russia_316', 'russia_317', 'russia_329', 'russia_344', 'russia_361', 'russia_366', 'russia_370', 'russia_371', 'russia_373', 'russia_380', 'russia_399', 'russia_400', 'russia_401', 'russia_405', 'russia_411', 'russia_413', 'russia_415', 'russia_433', 'russia_440', 'russia_445', 'russia_455', 'russia_481', 'russia_497']</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>56</v>
+      </c>
+      <c r="H4" t="n">
+        <v>96</v>
+      </c>
+      <c r="I4" t="n">
+        <v>99</v>
       </c>
     </row>
     <row r="5">
@@ -521,13 +603,32 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['russia_28', 'russia_115', 'russia_118', 'russia_189', 'russia_191', 'russia_259', 'russia_384']</t>
+          <t>['russia_189']</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>['russia_10', 'russia_12', 'russia_13', 'russia_15', 'russia_16', 'russia_19', 'russia_28', 'russia_31', 'russia_89', 'russia_90', 'russia_115', 'russia_118', 'russia_150', 'russia_183', 'russia_188', 'russia_190', 'russia_191', 'russia_192', 'russia_194', 'russia_198', 'russia_228', 'russia_242', 'russia_259', 'russia_260', 'russia_261', 'russia_264', 'russia_330', 'russia_351', 'russia_379', 'russia_383', 'russia_384', 'russia_386', 'russia_409', 'russia_430', 'russia_444', 'russia_488']</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>['russia_93', 'russia_363']</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>37</v>
+      </c>
+      <c r="H5" t="n">
+        <v>283</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -541,13 +642,32 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['russia_189']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>['russia_115', 'russia_118', 'russia_189', 'russia_198', 'russia_330', 'russia_384', 'russia_409']</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>7</v>
+      </c>
+      <c r="H6" t="n">
+        <v>327</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -569,6 +689,25 @@
           <t>[]</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" t="n">
+        <v>345</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -581,13 +720,32 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['russia_3', 'russia_4', 'russia_23', 'russia_29', 'russia_46', 'russia_48', 'russia_88', 'russia_115', 'russia_328', 'russia_344']</t>
+          <t>['russia_4', 'russia_23', 'russia_48', 'russia_88', 'russia_115', 'russia_328']</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>['russia_56', 'russia_181']</t>
         </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>['russia_3', 'russia_29', 'russia_45', 'russia_46', 'russia_57', 'russia_111', 'russia_316', 'russia_344', 'russia_361']</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>['russia_108', 'russia_156', 'russia_470']</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>15</v>
+      </c>
+      <c r="H8" t="n">
+        <v>297</v>
+      </c>
+      <c r="I8" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -609,6 +767,25 @@
           <t>[]</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>['russia_156']</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" t="n">
+        <v>376</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -621,13 +798,32 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>['russia_1', 'russia_11', 'russia_17', 'russia_21', 'russia_23', 'russia_24', 'russia_26', 'russia_27', 'russia_29', 'russia_34', 'russia_37', 'russia_38', 'russia_42', 'russia_46', 'russia_51', 'russia_57', 'russia_63', 'russia_65', 'russia_69', 'russia_71', 'russia_80', 'russia_83', 'russia_84', 'russia_87', 'russia_98', 'russia_99', 'russia_103', 'russia_106', 'russia_107', 'russia_110', 'russia_111', 'russia_125', 'russia_132', 'russia_138', 'russia_152', 'russia_154', 'russia_155', 'russia_157', 'russia_158', 'russia_183', 'russia_200', 'russia_209', 'russia_214', 'russia_220', 'russia_222', 'russia_223', 'russia_224', 'russia_225', 'russia_226', 'russia_227', 'russia_228', 'russia_229', 'russia_233', 'russia_234', 'russia_235', 'russia_238', 'russia_242', 'russia_252', 'russia_256', 'russia_258', 'russia_260', 'russia_262', 'russia_264', 'russia_266', 'russia_267', 'russia_271', 'russia_274', 'russia_283', 'russia_287', 'russia_289', 'russia_293', 'russia_294', 'russia_300', 'russia_301', 'russia_305', 'russia_306', 'russia_319', 'russia_328', 'russia_331', 'russia_334', 'russia_335', 'russia_337', 'russia_344', 'russia_346', 'russia_358', 'russia_359', 'russia_361', 'russia_364', 'russia_370', 'russia_372', 'russia_373', 'russia_374', 'russia_379', 'russia_380', 'russia_392', 'russia_394', 'russia_395', 'russia_399', 'russia_403', 'russia_404', 'russia_405', 'russia_413', 'russia_414', 'russia_415', 'russia_417', 'russia_421', 'russia_422', 'russia_424', 'russia_425', 'russia_428', 'russia_433', 'russia_434', 'russia_435', 'russia_440', 'russia_443', 'russia_445', 'russia_448', 'russia_453', 'russia_458', 'russia_459', 'russia_461', 'russia_468', 'russia_469', 'russia_480', 'russia_481', 'russia_483', 'russia_486', 'russia_491', 'russia_495', 'russia_497', 'russia_499']</t>
+          <t>['russia_11', 'russia_17', 'russia_21', 'russia_23', 'russia_24', 'russia_26', 'russia_27', 'russia_29', 'russia_34', 'russia_37', 'russia_38', 'russia_42', 'russia_46', 'russia_63', 'russia_69', 'russia_71', 'russia_80', 'russia_83', 'russia_84', 'russia_87', 'russia_98', 'russia_99', 'russia_103', 'russia_106', 'russia_107', 'russia_110', 'russia_111', 'russia_132', 'russia_138', 'russia_152', 'russia_154', 'russia_155', 'russia_157', 'russia_158', 'russia_200', 'russia_209', 'russia_214', 'russia_220', 'russia_222', 'russia_223', 'russia_224', 'russia_225', 'russia_226', 'russia_227', 'russia_228', 'russia_229', 'russia_233', 'russia_234', 'russia_235', 'russia_238', 'russia_242', 'russia_252', 'russia_256', 'russia_260', 'russia_262', 'russia_264', 'russia_266', 'russia_267', 'russia_271', 'russia_274', 'russia_283', 'russia_287', 'russia_289', 'russia_293', 'russia_294', 'russia_300', 'russia_301', 'russia_305', 'russia_306', 'russia_319', 'russia_328', 'russia_331', 'russia_334', 'russia_335', 'russia_337', 'russia_344', 'russia_358', 'russia_359', 'russia_361', 'russia_364', 'russia_370', 'russia_372', 'russia_373', 'russia_374', 'russia_380', 'russia_392', 'russia_394', 'russia_395', 'russia_399', 'russia_403', 'russia_404', 'russia_405', 'russia_413', 'russia_414', 'russia_415', 'russia_417', 'russia_421', 'russia_422', 'russia_424', 'russia_425', 'russia_428', 'russia_433', 'russia_434', 'russia_435', 'russia_443', 'russia_445', 'russia_448', 'russia_458', 'russia_459', 'russia_468', 'russia_469', 'russia_480', 'russia_483', 'russia_486', 'russia_491', 'russia_495', 'russia_497', 'russia_499']</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>['russia_1', 'russia_7', 'russia_28', 'russia_44', 'russia_48', 'russia_51', 'russia_57', 'russia_65', 'russia_89', 'russia_90', 'russia_125', 'russia_133', 'russia_139', 'russia_183', 'russia_258', 'russia_346', 'russia_351', 'russia_360', 'russia_379', 'russia_400', 'russia_409', 'russia_427', 'russia_440', 'russia_453', 'russia_454', 'russia_455', 'russia_457', 'russia_461', 'russia_481']</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>['russia_156']</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>147</v>
+      </c>
+      <c r="H10" t="n">
+        <v>212</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -641,13 +837,32 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>['russia_10', 'russia_19', 'russia_28', 'russia_40', 'russia_43', 'russia_68', 'russia_112', 'russia_115', 'russia_120', 'russia_144', 'russia_154', 'russia_188', 'russia_192', 'russia_195', 'russia_260', 'russia_273', 'russia_300', 'russia_319', 'russia_340', 'russia_342', 'russia_347', 'russia_351', 'russia_409']</t>
+          <t>['russia_19', 'russia_40', 'russia_154', 'russia_195', 'russia_300', 'russia_342', 'russia_347', 'russia_351', 'russia_409']</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>['russia_61', 'russia_108', 'russia_156', 'russia_285', 'russia_315', 'russia_345', 'russia_363', 'russia_476']</t>
-        </is>
+          <t>['russia_108', 'russia_363']</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>['russia_9', 'russia_10', 'russia_13', 'russia_28', 'russia_43', 'russia_68', 'russia_100', 'russia_106', 'russia_112', 'russia_115', 'russia_118', 'russia_120', 'russia_144', 'russia_150', 'russia_158', 'russia_187', 'russia_188', 'russia_189', 'russia_190', 'russia_191', 'russia_192', 'russia_194', 'russia_198', 'russia_235', 'russia_242', 'russia_252', 'russia_258', 'russia_259', 'russia_260', 'russia_261', 'russia_264', 'russia_273', 'russia_279', 'russia_309', 'russia_319', 'russia_330', 'russia_332', 'russia_334', 'russia_340', 'russia_377', 'russia_384', 'russia_390', 'russia_444', 'russia_457', 'russia_488']</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>['russia_20', 'russia_49', 'russia_61', 'russia_70', 'russia_138', 'russia_156', 'russia_285', 'russia_315', 'russia_345', 'russia_476']</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>54</v>
+      </c>
+      <c r="H11" t="n">
+        <v>200</v>
+      </c>
+      <c r="I11" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -666,8 +881,27 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>['russia_62', 'russia_64', 'russia_75', 'russia_138']</t>
-        </is>
+          <t>['russia_75', 'russia_138']</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>['russia_35', 'russia_50', 'russia_62', 'russia_64', 'russia_81', 'russia_210', 'russia_271', 'russia_303', 'russia_322', 'russia_325', 'russia_366']</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>323</v>
+      </c>
+      <c r="I12" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="13">
@@ -689,6 +923,25 @@
           <t>['russia_156']</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>['russia_118', 'russia_142']</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" t="n">
+        <v>348</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -701,13 +954,32 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>['russia_23', 'russia_29', 'russia_38', 'russia_57', 'russia_69', 'russia_95', 'russia_119', 'russia_132', 'russia_135', 'russia_144', 'russia_149', 'russia_158', 'russia_175', 'russia_195', 'russia_200', 'russia_262', 'russia_274', 'russia_310', 'russia_317', 'russia_321', 'russia_342', 'russia_344', 'russia_356', 'russia_363', 'russia_372', 'russia_373', 'russia_414', 'russia_415', 'russia_434', 'russia_454', 'russia_458', 'russia_459']</t>
+          <t>['russia_38', 'russia_57', 'russia_69', 'russia_95', 'russia_119', 'russia_135', 'russia_149', 'russia_158', 'russia_195', 'russia_274', 'russia_310', 'russia_317', 'russia_342', 'russia_344', 'russia_356', 'russia_372', 'russia_373', 'russia_415', 'russia_434', 'russia_454', 'russia_458', 'russia_459']</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>['russia_11', 'russia_23', 'russia_29', 'russia_132', 'russia_144', 'russia_175', 'russia_200', 'russia_252', 'russia_262', 'russia_266', 'russia_321', 'russia_340', 'russia_363', 'russia_370', 'russia_409', 'russia_414', 'russia_461', 'russia_468']</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>40</v>
+      </c>
+      <c r="H14" t="n">
+        <v>321</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -721,13 +993,32 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>['russia_3', 'russia_13', 'russia_19', 'russia_23', 'russia_28', 'russia_45', 'russia_46', 'russia_83', 'russia_87', 'russia_88', 'russia_89', 'russia_105', 'russia_106', 'russia_115', 'russia_118', 'russia_135', 'russia_144', 'russia_149', 'russia_154', 'russia_158', 'russia_159', 'russia_175', 'russia_183', 'russia_188', 'russia_189', 'russia_193', 'russia_194', 'russia_198', 'russia_223', 'russia_229', 'russia_233', 'russia_242', 'russia_257', 'russia_263', 'russia_277', 'russia_281', 'russia_301', 'russia_307', 'russia_309', 'russia_315', 'russia_330', 'russia_340', 'russia_341', 'russia_342', 'russia_347', 'russia_356', 'russia_358', 'russia_360', 'russia_368', 'russia_383', 'russia_396', 'russia_409', 'russia_444', 'russia_448', 'russia_458', 'russia_459', 'russia_462', 'russia_464']</t>
+          <t>['russia_13', 'russia_19', 'russia_23', 'russia_45', 'russia_46', 'russia_88', 'russia_89', 'russia_115', 'russia_144', 'russia_149', 'russia_158', 'russia_159', 'russia_188', 'russia_198', 'russia_229', 'russia_257', 'russia_263', 'russia_281', 'russia_301', 'russia_309', 'russia_340', 'russia_341', 'russia_342', 'russia_347', 'russia_356', 'russia_358', 'russia_360', 'russia_383', 'russia_448', 'russia_459', 'russia_462', 'russia_464']</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>['russia_8', 'russia_61', 'russia_108', 'russia_156', 'russia_219']</t>
-        </is>
+          <t>['russia_108', 'russia_219']</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>['russia_3', 'russia_4', 'russia_18', 'russia_28', 'russia_29', 'russia_48', 'russia_59', 'russia_67', 'russia_68', 'russia_83', 'russia_87', 'russia_90', 'russia_100', 'russia_101', 'russia_105', 'russia_106', 'russia_117', 'russia_118', 'russia_135', 'russia_137', 'russia_154', 'russia_175', 'russia_181', 'russia_183', 'russia_187', 'russia_189', 'russia_191', 'russia_192', 'russia_193', 'russia_194', 'russia_195', 'russia_213', 'russia_223', 'russia_226', 'russia_228', 'russia_233', 'russia_235', 'russia_237', 'russia_242', 'russia_254', 'russia_259', 'russia_260', 'russia_261', 'russia_277', 'russia_279', 'russia_296', 'russia_307', 'russia_315', 'russia_317', 'russia_319', 'russia_330', 'russia_331', 'russia_334', 'russia_337', 'russia_348', 'russia_351', 'russia_364', 'russia_368', 'russia_377', 'russia_379', 'russia_384', 'russia_396', 'russia_409', 'russia_430', 'russia_437', 'russia_438', 'russia_444', 'russia_453', 'russia_457', 'russia_458', 'russia_480', 'russia_488', 'russia_500']</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>['russia_8', 'russia_49', 'russia_56', 'russia_61', 'russia_62', 'russia_70', 'russia_93', 'russia_112', 'russia_138', 'russia_156', 'russia_180', 'russia_285', 'russia_303', 'russia_322', 'russia_363', 'russia_366', 'russia_476']</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>105</v>
+      </c>
+      <c r="H15" t="n">
+        <v>99</v>
+      </c>
+      <c r="I15" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="16">
@@ -741,13 +1032,32 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>['russia_6', 'russia_19', 'russia_31', 'russia_235', 'russia_260', 'russia_316', 'russia_346', 'russia_350', 'russia_371', 'russia_386', 'russia_493', 'russia_497', 'russia_501']</t>
+          <t>['russia_6', 'russia_316', 'russia_346', 'russia_371', 'russia_386', 'russia_493', 'russia_497', 'russia_501']</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>['russia_8', 'russia_24', 'russia_25', 'russia_38', 'russia_43', 'russia_81', 'russia_112', 'russia_114', 'russia_138', 'russia_156', 'russia_159', 'russia_175', 'russia_176', 'russia_180', 'russia_209', 'russia_211', 'russia_214', 'russia_216', 'russia_217', 'russia_234', 'russia_240', 'russia_252', 'russia_271', 'russia_273', 'russia_299', 'russia_300', 'russia_309', 'russia_310', 'russia_321', 'russia_344', 'russia_363', 'russia_369', 'russia_370', 'russia_403', 'russia_407', 'russia_411', 'russia_424', 'russia_425', 'russia_436', 'russia_440', 'russia_454', 'russia_476', 'russia_477', 'russia_478', 'russia_490']</t>
-        </is>
+          <t>['russia_43', 'russia_112', 'russia_138', 'russia_156', 'russia_159', 'russia_175', 'russia_176', 'russia_180', 'russia_211', 'russia_252', 'russia_273', 'russia_300', 'russia_363', 'russia_369', 'russia_403', 'russia_407', 'russia_424', 'russia_425', 'russia_454', 'russia_476']</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>['russia_19', 'russia_31', 'russia_65', 'russia_89', 'russia_90', 'russia_98', 'russia_106', 'russia_115', 'russia_118', 'russia_183', 'russia_191', 'russia_222', 'russia_235', 'russia_237', 'russia_242', 'russia_260', 'russia_334', 'russia_348', 'russia_350', 'russia_384', 'russia_409', 'russia_444']</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>['russia_4', 'russia_8', 'russia_11', 'russia_17', 'russia_20', 'russia_23', 'russia_24', 'russia_25', 'russia_35', 'russia_36', 'russia_38', 'russia_50', 'russia_57', 'russia_61', 'russia_62', 'russia_63', 'russia_69', 'russia_70', 'russia_71', 'russia_81', 'russia_94', 'russia_97', 'russia_108', 'russia_114', 'russia_117', 'russia_132', 'russia_133', 'russia_142', 'russia_144', 'russia_149', 'russia_154', 'russia_157', 'russia_177', 'russia_195', 'russia_209', 'russia_214', 'russia_216', 'russia_217', 'russia_233', 'russia_234', 'russia_240', 'russia_253', 'russia_254', 'russia_262', 'russia_266', 'russia_271', 'russia_274', 'russia_279', 'russia_294', 'russia_299', 'russia_301', 'russia_303', 'russia_305', 'russia_306', 'russia_308', 'russia_309', 'russia_310', 'russia_313', 'russia_317', 'russia_321', 'russia_322', 'russia_323', 'russia_340', 'russia_342', 'russia_344', 'russia_362', 'russia_364', 'russia_368', 'russia_370', 'russia_388', 'russia_392', 'russia_399', 'russia_405', 'russia_411', 'russia_414', 'russia_422', 'russia_433', 'russia_434', 'russia_436', 'russia_438', 'russia_440', 'russia_468', 'russia_470', 'russia_473', 'russia_475', 'russia_477', 'russia_478', 'russia_481', 'russia_482', 'russia_486', 'russia_490', 'russia_495', 'russia_499']</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>30</v>
+      </c>
+      <c r="H16" t="n">
+        <v>75</v>
+      </c>
+      <c r="I16" t="n">
+        <v>113</v>
       </c>
     </row>
     <row r="17">
@@ -769,6 +1079,25 @@
           <t>[]</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>['russia_409']</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>['russia_313']</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" t="n">
+        <v>336</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -781,13 +1110,32 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>['russia_11', 'russia_19', 'russia_20', 'russia_28', 'russia_150', 'russia_198']</t>
+          <t>['russia_11', 'russia_20', 'russia_198']</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>['russia_13', 'russia_15', 'russia_16', 'russia_19', 'russia_28', 'russia_29', 'russia_46', 'russia_89', 'russia_106', 'russia_118', 'russia_150', 'russia_183', 'russia_187', 'russia_189', 'russia_191', 'russia_237', 'russia_241', 'russia_259', 'russia_264', 'russia_330', 'russia_334', 'russia_347', 'russia_348', 'russia_384', 'russia_386', 'russia_409', 'russia_444', 'russia_462', 'russia_500']</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>['russia_61', 'russia_316', 'russia_361']</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>32</v>
+      </c>
+      <c r="H18" t="n">
+        <v>166</v>
+      </c>
+      <c r="I18" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -801,13 +1149,32 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>['russia_17', 'russia_19', 'russia_399']</t>
+          <t>['russia_17', 'russia_399']</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>['russia_23', 'russia_38', 'russia_57', 'russia_69', 'russia_81', 'russia_114', 'russia_117', 'russia_154', 'russia_175', 'russia_180', 'russia_234', 'russia_252', 'russia_273', 'russia_294', 'russia_301', 'russia_315', 'russia_323', 'russia_363', 'russia_366', 'russia_438', 'russia_494']</t>
-        </is>
+          <t>['russia_38', 'russia_154', 'russia_175', 'russia_234', 'russia_301']</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>['russia_19', 'russia_28', 'russia_118', 'russia_198', 'russia_255', 'russia_304', 'russia_348', 'russia_392']</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>['russia_4', 'russia_8', 'russia_23', 'russia_24', 'russia_25', 'russia_26', 'russia_43', 'russia_45', 'russia_57', 'russia_61', 'russia_69', 'russia_74', 'russia_81', 'russia_94', 'russia_95', 'russia_99', 'russia_108', 'russia_111', 'russia_114', 'russia_117', 'russia_132', 'russia_138', 'russia_151', 'russia_158', 'russia_159', 'russia_180', 'russia_181', 'russia_214', 'russia_252', 'russia_266', 'russia_273', 'russia_274', 'russia_294', 'russia_305', 'russia_315', 'russia_317', 'russia_321', 'russia_322', 'russia_323', 'russia_340', 'russia_344', 'russia_361', 'russia_363', 'russia_366', 'russia_369', 'russia_370', 'russia_388', 'russia_405', 'russia_407', 'russia_422', 'russia_433', 'russia_438', 'russia_445', 'russia_470', 'russia_481', 'russia_494']</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>10</v>
+      </c>
+      <c r="H19" t="n">
+        <v>181</v>
+      </c>
+      <c r="I19" t="n">
+        <v>61</v>
       </c>
     </row>
     <row r="20">
@@ -829,6 +1196,25 @@
           <t>[]</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>2</v>
+      </c>
+      <c r="H20" t="n">
+        <v>361</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -846,8 +1232,27 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>['russia_112', 'russia_144', 'russia_181', 'russia_366', 'russia_458']</t>
-        </is>
+          <t>['russia_144', 'russia_181']</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>['russia_23']</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>['russia_20', 'russia_54', 'russia_56', 'russia_70', 'russia_112', 'russia_366', 'russia_458', 'russia_470', 'russia_476']</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" t="n">
+        <v>330</v>
+      </c>
+      <c r="I21" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="22">
@@ -861,13 +1266,32 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>['russia_29', 'russia_69', 'russia_198', 'russia_356']</t>
+          <t>['russia_29', 'russia_356']</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
           <t>['russia_325']</t>
         </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>['russia_38', 'russia_69', 'russia_198']</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>['russia_70', 'russia_366']</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>5</v>
+      </c>
+      <c r="H22" t="n">
+        <v>357</v>
+      </c>
+      <c r="I22" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="23">
@@ -886,8 +1310,27 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>['russia_43', 'russia_61', 'russia_112', 'russia_117', 'russia_137', 'russia_138', 'russia_156', 'russia_176', 'russia_180', 'russia_213', 'russia_219', 'russia_294', 'russia_299', 'russia_315', 'russia_363', 'russia_366', 'russia_401', 'russia_411', 'russia_436', 'russia_478']</t>
-        </is>
+          <t>['russia_112', 'russia_137', 'russia_176', 'russia_180', 'russia_219', 'russia_294', 'russia_315', 'russia_478']</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>['russia_19', 'russia_28', 'russia_118', 'russia_409']</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>['russia_4', 'russia_8', 'russia_26', 'russia_38', 'russia_43', 'russia_49', 'russia_56', 'russia_61', 'russia_74', 'russia_93', 'russia_105', 'russia_117', 'russia_132', 'russia_136', 'russia_138', 'russia_143', 'russia_149', 'russia_154', 'russia_156', 'russia_196', 'russia_210', 'russia_213', 'russia_217', 'russia_220', 'russia_240', 'russia_252', 'russia_299', 'russia_303', 'russia_305', 'russia_322', 'russia_345', 'russia_363', 'russia_364', 'russia_366', 'russia_368', 'russia_401', 'russia_411', 'russia_422', 'russia_436', 'russia_438', 'russia_455', 'russia_476', 'russia_477']</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>4</v>
+      </c>
+      <c r="H23" t="n">
+        <v>233</v>
+      </c>
+      <c r="I23" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="24">
@@ -906,8 +1349,27 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>['russia_37', 'russia_157', 'russia_176', 'russia_274']</t>
-        </is>
+          <t>['russia_37', 'russia_157']</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>['russia_28', 'russia_409']</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>['russia_156', 'russia_176', 'russia_210', 'russia_274', 'russia_303', 'russia_322', 'russia_323', 'russia_436']</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>2</v>
+      </c>
+      <c r="H24" t="n">
+        <v>315</v>
+      </c>
+      <c r="I24" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="25">
@@ -921,13 +1383,32 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>['russia_307', 'russia_314', 'russia_360']</t>
+          <t>['russia_360']</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>['russia_28', 'russia_307', 'russia_314', 'russia_453']</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>['russia_139', 'russia_156', 'russia_266']</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>5</v>
+      </c>
+      <c r="H25" t="n">
+        <v>351</v>
+      </c>
+      <c r="I25" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="26">
@@ -941,13 +1422,32 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>['russia_54', 'russia_141', 'russia_144', 'russia_307']</t>
+          <t>['russia_54', 'russia_141']</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>['russia_49', 'russia_56', 'russia_61', 'russia_81', 'russia_114', 'russia_138', 'russia_156', 'russia_219', 'russia_285', 'russia_325', 'russia_371', 'russia_476', 'russia_485', 'russia_497', 'russia_498']</t>
-        </is>
+          <t>['russia_56', 'russia_61', 'russia_156', 'russia_219', 'russia_325', 'russia_476', 'russia_485', 'russia_497', 'russia_498']</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>['russia_28', 'russia_118', 'russia_144', 'russia_307', 'russia_444']</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>['russia_14', 'russia_17', 'russia_20', 'russia_25', 'russia_49', 'russia_53', 'russia_81', 'russia_93', 'russia_94', 'russia_114', 'russia_138', 'russia_139', 'russia_176', 'russia_180', 'russia_210', 'russia_217', 'russia_221', 'russia_234', 'russia_253', 'russia_255', 'russia_269', 'russia_279', 'russia_285', 'russia_297', 'russia_302', 'russia_329', 'russia_371', 'russia_463']</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>7</v>
+      </c>
+      <c r="H26" t="n">
+        <v>247</v>
+      </c>
+      <c r="I26" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="27">
@@ -966,8 +1466,27 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>['russia_62', 'russia_99', 'russia_176', 'russia_210', 'russia_316', 'russia_401']</t>
-        </is>
+          <t>['russia_62', 'russia_316', 'russia_401']</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>['russia_99', 'russia_154', 'russia_176', 'russia_210', 'russia_287', 'russia_405', 'russia_411', 'russia_455', 'russia_498']</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" t="n">
+        <v>327</v>
+      </c>
+      <c r="I27" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="28">
@@ -986,8 +1505,27 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>['russia_409']</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
           <t>['russia_70']</t>
         </is>
+      </c>
+      <c r="G28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H28" t="n">
+        <v>361</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -1006,8 +1544,27 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>['russia_61', 'russia_114', 'russia_156', 'russia_219', 'russia_253', 'russia_273']</t>
-        </is>
+          <t>['russia_61', 'russia_156', 'russia_219']</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>['russia_28', 'russia_118', 'russia_198', 'russia_262', 'russia_370', 'russia_407']</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>['russia_8', 'russia_26', 'russia_74', 'russia_93', 'russia_94', 'russia_114', 'russia_117', 'russia_136', 'russia_138', 'russia_217', 'russia_253', 'russia_273', 'russia_303', 'russia_316', 'russia_363', 'russia_401', 'russia_470', 'russia_476', 'russia_497']</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>6</v>
+      </c>
+      <c r="H29" t="n">
+        <v>295</v>
+      </c>
+      <c r="I29" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="30">
@@ -1021,13 +1578,32 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>['russia_84', 'russia_426', 'russia_434']</t>
+          <t>['russia_84', 'russia_426']</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>['russia_316']</t>
-        </is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>['russia_19', 'russia_28', 'russia_89', 'russia_106', 'russia_118', 'russia_187', 'russia_189', 'russia_299', 'russia_409', 'russia_418', 'russia_428', 'russia_430', 'russia_434', 'russia_436', 'russia_437', 'russia_444', 'russia_469']</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>['russia_4', 'russia_273', 'russia_300', 'russia_316', 'russia_321', 'russia_359', 'russia_497']</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>19</v>
+      </c>
+      <c r="H30" t="n">
+        <v>253</v>
+      </c>
+      <c r="I30" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="31">
@@ -1041,13 +1617,32 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>['russia_19', 'russia_115', 'russia_444']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>['russia_19', 'russia_28', 'russia_115', 'russia_118', 'russia_150', 'russia_189', 'russia_330', 'russia_348', 'russia_383', 'russia_384', 'russia_409', 'russia_444', 'russia_488']</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>['russia_61', 'russia_470']</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>13</v>
+      </c>
+      <c r="H31" t="n">
+        <v>300</v>
+      </c>
+      <c r="I31" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -1061,13 +1656,32 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>['russia_198']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>['russia_61', 'russia_71', 'russia_81', 'russia_98', 'russia_99', 'russia_155', 'russia_156', 'russia_180', 'russia_210', 'russia_445', 'russia_455']</t>
-        </is>
+          <t>['russia_61', 'russia_71', 'russia_99', 'russia_155', 'russia_180', 'russia_210', 'russia_445']</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>['russia_19', 'russia_28', 'russia_118', 'russia_190', 'russia_194', 'russia_198', 'russia_409']</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>['russia_8', 'russia_43', 'russia_81', 'russia_98', 'russia_101', 'russia_117', 'russia_141', 'russia_156', 'russia_181', 'russia_226', 'russia_234', 'russia_273', 'russia_303', 'russia_316', 'russia_364', 'russia_417', 'russia_455', 'russia_468']</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>7</v>
+      </c>
+      <c r="H32" t="n">
+        <v>272</v>
+      </c>
+      <c r="I32" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="33">
@@ -1081,13 +1695,32 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>['russia_19', 'russia_454']</t>
+          <t>['russia_454']</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>['russia_1', 'russia_3', 'russia_4', 'russia_8', 'russia_11', 'russia_14', 'russia_17', 'russia_20', 'russia_21', 'russia_22', 'russia_23', 'russia_24', 'russia_25', 'russia_26', 'russia_29', 'russia_34', 'russia_35', 'russia_36', 'russia_38', 'russia_43', 'russia_48', 'russia_50', 'russia_51', 'russia_56', 'russia_57', 'russia_58', 'russia_61', 'russia_62', 'russia_66', 'russia_68', 'russia_69', 'russia_70', 'russia_75', 'russia_77', 'russia_80', 'russia_81', 'russia_84', 'russia_88', 'russia_95', 'russia_97', 'russia_99', 'russia_103', 'russia_105', 'russia_108', 'russia_112', 'russia_114', 'russia_133', 'russia_135', 'russia_136', 'russia_137', 'russia_138', 'russia_141', 'russia_142', 'russia_143', 'russia_144', 'russia_149', 'russia_152', 'russia_154', 'russia_156', 'russia_157', 'russia_158', 'russia_159', 'russia_175', 'russia_176', 'russia_177', 'russia_180', 'russia_181', 'russia_182', 'russia_195', 'russia_209', 'russia_210', 'russia_211', 'russia_212', 'russia_213', 'russia_214', 'russia_217', 'russia_218', 'russia_219', 'russia_220', 'russia_221', 'russia_224', 'russia_225', 'russia_227', 'russia_229', 'russia_231', 'russia_233', 'russia_234', 'russia_239', 'russia_240', 'russia_241', 'russia_252', 'russia_253', 'russia_256', 'russia_257', 'russia_262', 'russia_263', 'russia_271', 'russia_273', 'russia_274', 'russia_275', 'russia_277', 'russia_279', 'russia_285', 'russia_287', 'russia_289', 'russia_294', 'russia_297', 'russia_298', 'russia_299', 'russia_301', 'russia_304', 'russia_305', 'russia_306', 'russia_309', 'russia_310', 'russia_314', 'russia_315', 'russia_316', 'russia_317', 'russia_321', 'russia_322', 'russia_323', 'russia_328', 'russia_329', 'russia_340', 'russia_341', 'russia_342', 'russia_344', 'russia_345', 'russia_346', 'russia_350', 'russia_359', 'russia_362', 'russia_363', 'russia_364', 'russia_366', 'russia_367', 'russia_368', 'russia_369', 'russia_370', 'russia_371', 'russia_372', 'russia_373', 'russia_374', 'russia_380', 'russia_388', 'russia_392', 'russia_396', 'russia_399', 'russia_400', 'russia_401', 'russia_403', 'russia_405', 'russia_407', 'russia_411', 'russia_413', 'russia_414', 'russia_415', 'russia_418', 'russia_422', 'russia_424', 'russia_425', 'russia_426', 'russia_431', 'russia_433', 'russia_434', 'russia_435', 'russia_436', 'russia_438', 'russia_440', 'russia_453', 'russia_455', 'russia_461', 'russia_467', 'russia_468', 'russia_469', 'russia_473', 'russia_475', 'russia_476', 'russia_477', 'russia_478', 'russia_481', 'russia_483', 'russia_485', 'russia_486', 'russia_490', 'russia_495', 'russia_497', 'russia_498', 'russia_499']</t>
-        </is>
+          <t>['russia_4', 'russia_11', 'russia_14', 'russia_20', 'russia_21', 'russia_22', 'russia_24', 'russia_25', 'russia_26', 'russia_38', 'russia_43', 'russia_48', 'russia_50', 'russia_51', 'russia_56', 'russia_57', 'russia_61', 'russia_62', 'russia_66', 'russia_69', 'russia_75', 'russia_77', 'russia_80', 'russia_81', 'russia_84', 'russia_95', 'russia_97', 'russia_108', 'russia_112', 'russia_114', 'russia_133', 'russia_136', 'russia_137', 'russia_138', 'russia_141', 'russia_142', 'russia_144', 'russia_149', 'russia_152', 'russia_154', 'russia_157', 'russia_158', 'russia_159', 'russia_175', 'russia_176', 'russia_177', 'russia_180', 'russia_181', 'russia_209', 'russia_211', 'russia_212', 'russia_213', 'russia_214', 'russia_218', 'russia_219', 'russia_220', 'russia_224', 'russia_229', 'russia_231', 'russia_233', 'russia_234', 'russia_240', 'russia_252', 'russia_256', 'russia_257', 'russia_262', 'russia_263', 'russia_271', 'russia_273', 'russia_274', 'russia_277', 'russia_279', 'russia_294', 'russia_297', 'russia_298', 'russia_301', 'russia_304', 'russia_305', 'russia_309', 'russia_310', 'russia_315', 'russia_316', 'russia_317', 'russia_321', 'russia_322', 'russia_323', 'russia_329', 'russia_340', 'russia_341', 'russia_342', 'russia_344', 'russia_362', 'russia_363', 'russia_364', 'russia_368', 'russia_370', 'russia_371', 'russia_373', 'russia_388', 'russia_396', 'russia_399', 'russia_401', 'russia_407', 'russia_411', 'russia_413', 'russia_415', 'russia_418', 'russia_424', 'russia_425', 'russia_434', 'russia_436', 'russia_438', 'russia_440', 'russia_453', 'russia_461', 'russia_467', 'russia_473', 'russia_476', 'russia_478', 'russia_483', 'russia_486', 'russia_490', 'russia_495', 'russia_497', 'russia_498']</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>['russia_19', 'russia_28', 'russia_118', 'russia_198', 'russia_409', 'russia_437']</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>['russia_1', 'russia_3', 'russia_5', 'russia_8', 'russia_17', 'russia_23', 'russia_27', 'russia_29', 'russia_34', 'russia_35', 'russia_36', 'russia_45', 'russia_49', 'russia_53', 'russia_54', 'russia_58', 'russia_63', 'russia_68', 'russia_70', 'russia_71', 'russia_74', 'russia_76', 'russia_83', 'russia_88', 'russia_93', 'russia_94', 'russia_99', 'russia_100', 'russia_101', 'russia_102', 'russia_103', 'russia_105', 'russia_107', 'russia_111', 'russia_119', 'russia_132', 'russia_135', 'russia_143', 'russia_153', 'russia_155', 'russia_156', 'russia_182', 'russia_195', 'russia_196', 'russia_200', 'russia_210', 'russia_216', 'russia_217', 'russia_221', 'russia_222', 'russia_223', 'russia_225', 'russia_226', 'russia_227', 'russia_232', 'russia_235', 'russia_239', 'russia_241', 'russia_243', 'russia_253', 'russia_254', 'russia_266', 'russia_267', 'russia_268', 'russia_269', 'russia_272', 'russia_275', 'russia_281', 'russia_282', 'russia_285', 'russia_286', 'russia_287', 'russia_289', 'russia_293', 'russia_296', 'russia_299', 'russia_300', 'russia_303', 'russia_306', 'russia_307', 'russia_308', 'russia_313', 'russia_314', 'russia_328', 'russia_345', 'russia_346', 'russia_350', 'russia_356', 'russia_359', 'russia_360', 'russia_361', 'russia_366', 'russia_367', 'russia_369', 'russia_372', 'russia_374', 'russia_380', 'russia_387', 'russia_392', 'russia_400', 'russia_403', 'russia_404', 'russia_405', 'russia_412', 'russia_414', 'russia_416', 'russia_417', 'russia_422', 'russia_426', 'russia_431', 'russia_433', 'russia_435', 'russia_443', 'russia_455', 'russia_462', 'russia_464', 'russia_468', 'russia_469', 'russia_470', 'russia_475', 'russia_477', 'russia_481', 'russia_482', 'russia_485', 'russia_499']</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>7</v>
+      </c>
+      <c r="H33" t="n">
+        <v>38</v>
+      </c>
+      <c r="I33" t="n">
+        <v>250</v>
       </c>
     </row>
     <row r="34">
@@ -1101,13 +1734,32 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>['russia_97', 'russia_221']</t>
+          <t>['russia_97']</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>['russia_118', 'russia_216', 'russia_221', 'russia_409']</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>['russia_70', 'russia_94', 'russia_234', 'russia_285', 'russia_476']</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>5</v>
+      </c>
+      <c r="H34" t="n">
+        <v>327</v>
+      </c>
+      <c r="I34" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="35">
@@ -1129,6 +1781,25 @@
           <t>[]</t>
         </is>
       </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>['russia_28', 'russia_106', 'russia_118', 'russia_198', 'russia_348', 'russia_406', 'russia_409']</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>['russia_132', 'russia_303']</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>8</v>
+      </c>
+      <c r="H35" t="n">
+        <v>290</v>
+      </c>
+      <c r="I35" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1141,13 +1812,32 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>['russia_28', 'russia_118', 'russia_133', 'russia_145', 'russia_348']</t>
+          <t>['russia_145']</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>['russia_4', 'russia_34', 'russia_135', 'russia_240', 'russia_273', 'russia_294', 'russia_301', 'russia_310', 'russia_316', 'russia_363', 'russia_364', 'russia_370', 'russia_413', 'russia_438', 'russia_481', 'russia_483', 'russia_497']</t>
-        </is>
+          <t>['russia_4', 'russia_294', 'russia_363', 'russia_364']</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>['russia_13', 'russia_28', 'russia_89', 'russia_90', 'russia_106', 'russia_118', 'russia_133', 'russia_187', 'russia_188', 'russia_191', 'russia_194', 'russia_198', 'russia_259', 'russia_260', 'russia_261', 'russia_330', 'russia_334', 'russia_348', 'russia_383', 'russia_384', 'russia_406', 'russia_409', 'russia_428', 'russia_430', 'russia_444', 'russia_488']</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>['russia_3', 'russia_14', 'russia_23', 'russia_34', 'russia_38', 'russia_45', 'russia_88', 'russia_105', 'russia_112', 'russia_135', 'russia_144', 'russia_149', 'russia_154', 'russia_156', 'russia_157', 'russia_175', 'russia_209', 'russia_229', 'russia_240', 'russia_257', 'russia_273', 'russia_296', 'russia_301', 'russia_305', 'russia_309', 'russia_310', 'russia_315', 'russia_316', 'russia_340', 'russia_344', 'russia_345', 'russia_368', 'russia_370', 'russia_411', 'russia_413', 'russia_424', 'russia_425', 'russia_438', 'russia_440', 'russia_477', 'russia_478', 'russia_481', 'russia_483', 'russia_494', 'russia_497']</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>27</v>
+      </c>
+      <c r="H36" t="n">
+        <v>179</v>
+      </c>
+      <c r="I36" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="37">
@@ -1161,13 +1851,32 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>['russia_287', 'russia_307', 'russia_314', 'russia_360', 'russia_483']</t>
+          <t>['russia_360']</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>['russia_64', 'russia_156']</t>
-        </is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>['russia_287', 'russia_307', 'russia_314', 'russia_483']</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>['russia_64', 'russia_156', 'russia_176', 'russia_498']</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>5</v>
+      </c>
+      <c r="H37" t="n">
+        <v>364</v>
+      </c>
+      <c r="I37" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="38">
@@ -1186,8 +1895,27 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>['russia_22', 'russia_24', 'russia_43', 'russia_45', 'russia_63', 'russia_70', 'russia_76', 'russia_81', 'russia_97', 'russia_108', 'russia_112', 'russia_136', 'russia_138', 'russia_141', 'russia_156', 'russia_157', 'russia_159', 'russia_175', 'russia_176', 'russia_195', 'russia_212', 'russia_218', 'russia_219', 'russia_240', 'russia_268', 'russia_273', 'russia_274', 'russia_298', 'russia_300', 'russia_305', 'russia_316', 'russia_317', 'russia_321', 'russia_322', 'russia_323', 'russia_367', 'russia_368', 'russia_369', 'russia_371', 'russia_392', 'russia_401', 'russia_407', 'russia_411', 'russia_415', 'russia_424', 'russia_425', 'russia_454', 'russia_478', 'russia_490', 'russia_499']</t>
-        </is>
+          <t>['russia_45', 'russia_63', 'russia_97', 'russia_138', 'russia_141', 'russia_157', 'russia_159', 'russia_176', 'russia_195', 'russia_212', 'russia_218', 'russia_219', 'russia_240', 'russia_268', 'russia_298', 'russia_300', 'russia_316', 'russia_317', 'russia_321', 'russia_323', 'russia_367', 'russia_368', 'russia_392', 'russia_401', 'russia_407', 'russia_424', 'russia_425', 'russia_454', 'russia_490']</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>['russia_19', 'russia_28', 'russia_118', 'russia_260', 'russia_406', 'russia_409']</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>['russia_14', 'russia_22', 'russia_24', 'russia_43', 'russia_49', 'russia_56', 'russia_61', 'russia_70', 'russia_74', 'russia_76', 'russia_81', 'russia_93', 'russia_108', 'russia_112', 'russia_132', 'russia_133', 'russia_136', 'russia_144', 'russia_154', 'russia_156', 'russia_175', 'russia_213', 'russia_266', 'russia_273', 'russia_274', 'russia_299', 'russia_303', 'russia_305', 'russia_307', 'russia_310', 'russia_315', 'russia_322', 'russia_362', 'russia_369', 'russia_371', 'russia_403', 'russia_411', 'russia_415', 'russia_417', 'russia_436', 'russia_440', 'russia_455', 'russia_467', 'russia_468', 'russia_469', 'russia_473', 'russia_476', 'russia_478', 'russia_498', 'russia_499']</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>6</v>
+      </c>
+      <c r="H38" t="n">
+        <v>187</v>
+      </c>
+      <c r="I38" t="n">
+        <v>79</v>
       </c>
     </row>
     <row r="39">
@@ -1201,13 +1929,32 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>['russia_83', 'russia_118', 'russia_211', 'russia_252']</t>
+          <t>['russia_211', 'russia_252']</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>['russia_29', 'russia_61', 'russia_69', 'russia_93', 'russia_94', 'russia_125', 'russia_181', 'russia_232', 'russia_287', 'russia_313', 'russia_481']</t>
-        </is>
+          <t>['russia_61', 'russia_93']</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>['russia_28', 'russia_83', 'russia_89', 'russia_118', 'russia_192', 'russia_198', 'russia_330', 'russia_379', 'russia_383', 'russia_430', 'russia_444']</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>['russia_8', 'russia_26', 'russia_29', 'russia_53', 'russia_69', 'russia_94', 'russia_125', 'russia_136', 'russia_156', 'russia_181', 'russia_224', 'russia_232', 'russia_287', 'russia_313', 'russia_346', 'russia_361', 'russia_363', 'russia_481', 'russia_493']</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>13</v>
+      </c>
+      <c r="H39" t="n">
+        <v>288</v>
+      </c>
+      <c r="I39" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="40">
@@ -1226,8 +1973,27 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>['russia_70']</t>
-        </is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>['russia_490']</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>['russia_70', 'russia_253']</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>7</v>
+      </c>
+      <c r="H40" t="n">
+        <v>358</v>
+      </c>
+      <c r="I40" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -1241,13 +2007,32 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>['russia_19', 'russia_118', 'russia_330']</t>
+          <t>['russia_19']</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>['russia_20', 'russia_61', 'russia_93', 'russia_156', 'russia_176', 'russia_219', 'russia_221', 'russia_270', 'russia_294', 'russia_302', 'russia_303', 'russia_322', 'russia_363', 'russia_377', 'russia_403', 'russia_454', 'russia_476', 'russia_497']</t>
-        </is>
+          <t>['russia_20', 'russia_61', 'russia_156', 'russia_176', 'russia_219', 'russia_302', 'russia_363', 'russia_497']</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>['russia_10', 'russia_13', 'russia_16', 'russia_28', 'russia_44', 'russia_118', 'russia_187', 'russia_188', 'russia_189', 'russia_191', 'russia_258', 'russia_261', 'russia_330', 'russia_348', 'russia_383', 'russia_384', 'russia_409', 'russia_430', 'russia_444', 'russia_487', 'russia_488', 'russia_500']</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>['russia_8', 'russia_22', 'russia_23', 'russia_24', 'russia_57', 'russia_93', 'russia_94', 'russia_195', 'russia_212', 'russia_214', 'russia_216', 'russia_217', 'russia_221', 'russia_232', 'russia_266', 'russia_270', 'russia_288', 'russia_294', 'russia_299', 'russia_303', 'russia_306', 'russia_313', 'russia_315', 'russia_321', 'russia_322', 'russia_344', 'russia_361', 'russia_370', 'russia_377', 'russia_397', 'russia_403', 'russia_454', 'russia_455', 'russia_470', 'russia_476']</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>23</v>
+      </c>
+      <c r="H41" t="n">
+        <v>198</v>
+      </c>
+      <c r="I41" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="42">
@@ -1266,8 +2051,27 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>['russia_138', 'russia_217', 'russia_221']</t>
-        </is>
+          <t>['russia_138', 'russia_221']</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>['russia_217']</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>354</v>
+      </c>
+      <c r="I42" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="43">
@@ -1281,13 +2085,32 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>['russia_19', 'russia_224', 'russia_236']</t>
+          <t>['russia_224', 'russia_236']</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>['russia_3', 'russia_4', 'russia_20', 'russia_23', 'russia_48', 'russia_57', 'russia_61', 'russia_93', 'russia_95', 'russia_117', 'russia_144', 'russia_154', 'russia_175', 'russia_181', 'russia_212', 'russia_220', 'russia_223', 'russia_287', 'russia_303', 'russia_310', 'russia_316', 'russia_344', 'russia_366']</t>
-        </is>
+          <t>['russia_4', 'russia_20', 'russia_61', 'russia_154', 'russia_181']</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>['russia_19', 'russia_115', 'russia_118', 'russia_188', 'russia_189', 'russia_242', 'russia_330', 'russia_379', 'russia_409', 'russia_427']</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>['russia_3', 'russia_23', 'russia_29', 'russia_45', 'russia_48', 'russia_53', 'russia_54', 'russia_57', 'russia_74', 'russia_93', 'russia_94', 'russia_95', 'russia_112', 'russia_114', 'russia_117', 'russia_137', 'russia_141', 'russia_144', 'russia_149', 'russia_156', 'russia_158', 'russia_159', 'russia_175', 'russia_176', 'russia_195', 'russia_212', 'russia_220', 'russia_223', 'russia_252', 'russia_273', 'russia_277', 'russia_287', 'russia_301', 'russia_303', 'russia_310', 'russia_315', 'russia_316', 'russia_317', 'russia_322', 'russia_340', 'russia_344', 'russia_361', 'russia_366', 'russia_401', 'russia_436', 'russia_478']</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>12</v>
+      </c>
+      <c r="H43" t="n">
+        <v>184</v>
+      </c>
+      <c r="I43" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="44">
@@ -1301,13 +2124,32 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>['russia_19', 'russia_225', 'russia_409']</t>
+          <t>['russia_19', 'russia_225']</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>['russia_61', 'russia_81', 'russia_132', 'russia_137', 'russia_156', 'russia_158', 'russia_176', 'russia_181', 'russia_213', 'russia_271', 'russia_300', 'russia_315', 'russia_368', 'russia_401', 'russia_413', 'russia_438', 'russia_497']</t>
-        </is>
+          <t>['russia_61', 'russia_176', 'russia_181', 'russia_438']</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>['russia_28', 'russia_44', 'russia_115', 'russia_118', 'russia_187', 'russia_235', 'russia_237', 'russia_330', 'russia_334', 'russia_384', 'russia_409', 'russia_427']</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>['russia_8', 'russia_24', 'russia_25', 'russia_35', 'russia_70', 'russia_81', 'russia_95', 'russia_132', 'russia_133', 'russia_137', 'russia_138', 'russia_154', 'russia_156', 'russia_158', 'russia_180', 'russia_209', 'russia_210', 'russia_213', 'russia_220', 'russia_252', 'russia_271', 'russia_273', 'russia_274', 'russia_282', 'russia_287', 'russia_294', 'russia_300', 'russia_303', 'russia_310', 'russia_315', 'russia_363', 'russia_366', 'russia_368', 'russia_369', 'russia_399', 'russia_401', 'russia_405', 'russia_407', 'russia_411', 'russia_413', 'russia_415', 'russia_424', 'russia_425', 'russia_436', 'russia_455', 'russia_470', 'russia_476', 'russia_478', 'russia_494', 'russia_497']</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>14</v>
+      </c>
+      <c r="H44" t="n">
+        <v>205</v>
+      </c>
+      <c r="I44" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="45">
@@ -1329,6 +2171,25 @@
           <t>[]</t>
         </is>
       </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>['russia_118', 'russia_409']</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>3</v>
+      </c>
+      <c r="H45" t="n">
+        <v>317</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1349,6 +2210,25 @@
           <t>[]</t>
         </is>
       </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>['russia_118', 'russia_188', 'russia_194', 'russia_409', 'russia_430']</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>6</v>
+      </c>
+      <c r="H46" t="n">
+        <v>329</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1366,8 +2246,27 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>['russia_4', 'russia_24', 'russia_117', 'russia_156', 'russia_176', 'russia_181', 'russia_213', 'russia_220', 'russia_315', 'russia_325']</t>
-        </is>
+          <t>['russia_176', 'russia_181', 'russia_213', 'russia_325']</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>['russia_19', 'russia_89', 'russia_198', 'russia_237', 'russia_242', 'russia_384', 'russia_409']</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>['russia_4', 'russia_20', 'russia_23', 'russia_24', 'russia_94', 'russia_95', 'russia_112', 'russia_114', 'russia_117', 'russia_132', 'russia_138', 'russia_149', 'russia_154', 'russia_156', 'russia_175', 'russia_214', 'russia_220', 'russia_252', 'russia_257', 'russia_273', 'russia_277', 'russia_294', 'russia_303', 'russia_315', 'russia_317', 'russia_323', 'russia_361', 'russia_369', 'russia_415', 'russia_477', 'russia_478']</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>10</v>
+      </c>
+      <c r="H47" t="n">
+        <v>239</v>
+      </c>
+      <c r="I47" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="48">
@@ -1381,13 +2280,32 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>['russia_19', 'russia_118', 'russia_264', 'russia_409']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>['russia_4', 'russia_11', 'russia_20', 'russia_23', 'russia_24', 'russia_29', 'russia_43', 'russia_45', 'russia_48', 'russia_57', 'russia_69', 'russia_95', 'russia_112', 'russia_117', 'russia_132', 'russia_137', 'russia_144', 'russia_149', 'russia_154', 'russia_158', 'russia_159', 'russia_175', 'russia_181', 'russia_196', 'russia_212', 'russia_213', 'russia_220', 'russia_223', 'russia_273', 'russia_296', 'russia_301', 'russia_310', 'russia_315', 'russia_317', 'russia_321', 'russia_323', 'russia_344', 'russia_364', 'russia_368', 'russia_415', 'russia_438', 'russia_477', 'russia_478', 'russia_481']</t>
-        </is>
+          <t>['russia_11', 'russia_20', 'russia_23', 'russia_57', 'russia_69', 'russia_117', 'russia_144', 'russia_154', 'russia_158', 'russia_159', 'russia_181', 'russia_212', 'russia_213', 'russia_220', 'russia_315', 'russia_323', 'russia_344', 'russia_368', 'russia_438']</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>['russia_10', 'russia_19', 'russia_28', 'russia_44', 'russia_90', 'russia_118', 'russia_187', 'russia_188', 'russia_194', 'russia_198', 'russia_242', 'russia_260', 'russia_261', 'russia_264', 'russia_330', 'russia_379', 'russia_383', 'russia_384', 'russia_409', 'russia_427', 'russia_488']</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>['russia_3', 'russia_4', 'russia_22', 'russia_24', 'russia_29', 'russia_35', 'russia_40', 'russia_43', 'russia_45', 'russia_48', 'russia_61', 'russia_71', 'russia_93', 'russia_94', 'russia_95', 'russia_112', 'russia_125', 'russia_132', 'russia_137', 'russia_142', 'russia_149', 'russia_175', 'russia_176', 'russia_180', 'russia_196', 'russia_214', 'russia_223', 'russia_224', 'russia_266', 'russia_273', 'russia_274', 'russia_279', 'russia_294', 'russia_296', 'russia_297', 'russia_301', 'russia_305', 'russia_310', 'russia_316', 'russia_317', 'russia_321', 'russia_328', 'russia_340', 'russia_350', 'russia_361', 'russia_364', 'russia_366', 'russia_369', 'russia_373', 'russia_401', 'russia_405', 'russia_415', 'russia_445', 'russia_453', 'russia_475', 'russia_477', 'russia_478', 'russia_481']</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>21</v>
+      </c>
+      <c r="H48" t="n">
+        <v>166</v>
+      </c>
+      <c r="I48" t="n">
+        <v>77</v>
       </c>
     </row>
     <row r="49">
@@ -1409,6 +2327,25 @@
           <t>[]</t>
         </is>
       </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>['russia_19', 'russia_115', 'russia_118', 'russia_259', 'russia_379', 'russia_409']</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>['russia_61', 'russia_176', 'russia_303']</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>6</v>
+      </c>
+      <c r="H49" t="n">
+        <v>293</v>
+      </c>
+      <c r="I49" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1429,6 +2366,25 @@
           <t>[]</t>
         </is>
       </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>['russia_118', 'russia_409']</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>['russia_476']</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>3</v>
+      </c>
+      <c r="H50" t="n">
+        <v>325</v>
+      </c>
+      <c r="I50" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1441,13 +2397,32 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>['russia_360', 'russia_483']</t>
+          <t>['russia_483']</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>['russia_287', 'russia_307', 'russia_314', 'russia_360', 'russia_409']</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>['russia_61', 'russia_156', 'russia_176']</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>6</v>
+      </c>
+      <c r="H51" t="n">
+        <v>358</v>
+      </c>
+      <c r="I51" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="52">
@@ -1469,6 +2444,25 @@
           <t>[]</t>
         </is>
       </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>['russia_409']</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>4</v>
+      </c>
+      <c r="H52" t="n">
+        <v>328</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1486,8 +2480,27 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>['russia_45', 'russia_70', 'russia_71', 'russia_88', 'russia_99', 'russia_154', 'russia_156', 'russia_180', 'russia_225', 'russia_234', 'russia_266', 'russia_271', 'russia_285', 'russia_323', 'russia_345', 'russia_363', 'russia_366', 'russia_476']</t>
-        </is>
+          <t>['russia_180', 'russia_225', 'russia_234', 'russia_363', 'russia_366']</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>['russia_409']</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>['russia_8', 'russia_43', 'russia_45', 'russia_48', 'russia_49', 'russia_70', 'russia_71', 'russia_80', 'russia_81', 'russia_88', 'russia_95', 'russia_99', 'russia_105', 'russia_112', 'russia_138', 'russia_143', 'russia_152', 'russia_154', 'russia_156', 'russia_157', 'russia_210', 'russia_266', 'russia_270', 'russia_271', 'russia_285', 'russia_309', 'russia_322', 'russia_323', 'russia_340', 'russia_341', 'russia_342', 'russia_345', 'russia_364', 'russia_368', 'russia_369', 'russia_407', 'russia_411', 'russia_424', 'russia_425', 'russia_438', 'russia_455', 'russia_476', 'russia_477', 'russia_480', 'russia_481', 'russia_490', 'russia_497']</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>4</v>
+      </c>
+      <c r="H53" t="n">
+        <v>255</v>
+      </c>
+      <c r="I53" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="54">
@@ -1508,6 +2521,25 @@
         <is>
           <t>[]</t>
         </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>['russia_13', 'russia_28', 'russia_59', 'russia_118', 'russia_183', 'russia_188', 'russia_189', 'russia_191', 'russia_193', 'russia_194', 'russia_242', 'russia_258', 'russia_261', 'russia_330', 'russia_334', 'russia_351', 'russia_406', 'russia_409', 'russia_444', 'russia_500']</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>['russia_48', 'russia_61', 'russia_108', 'russia_224', 'russia_297']</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>23</v>
+      </c>
+      <c r="H54" t="n">
+        <v>266</v>
+      </c>
+      <c r="I54" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>